<commit_message>
update 2020/04/17 update Login
</commit_message>
<xml_diff>
--- a/doc/Matrix-SSM Shiro流程图.xlsx
+++ b/doc/Matrix-SSM Shiro流程图.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyWork\learnspace\my-github\matrix-ssm\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBC3032-662F-4D01-9CE8-54DC26E10A58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAFB7275-ED71-4819-8E1A-5C46F8641E55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shiro验证码验证流程" sheetId="1" r:id="rId1"/>
@@ -88,13 +88,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>552448</xdr:colOff>
+      <xdr:colOff>552447</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>133348</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>676274</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>57149</xdr:rowOff>
     </xdr:to>
@@ -111,8 +111,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2609848" y="1581148"/>
-          <a:ext cx="6991352" cy="4267201"/>
+          <a:off x="2609847" y="1581148"/>
+          <a:ext cx="7667627" cy="4267201"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -165,14 +165,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>619124</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>619125</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>271461</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>133348</xdr:rowOff>
     </xdr:to>
@@ -190,9 +190,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="6105524" y="447675"/>
-          <a:ext cx="1" cy="1133473"/>
+        <a:xfrm>
+          <a:off x="6419850" y="438150"/>
+          <a:ext cx="23811" cy="1142998"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1004,7 +1004,31 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>KAPTCHA_SESSION_KEY</a:t>
+            <a:t>KAPTCHA_SESSION_KEY[kaptcha</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>常量值</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>]</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="zh-CN" altLang="en-US" sz="1100">
@@ -1328,7 +1352,7 @@
       <xdr:row>27</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2648738" cy="474489"/>
+    <xdr:ext cx="3210815" cy="474489"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="32" name="文本框 31">
@@ -1342,8 +1366,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2419350" y="4962525"/>
-          <a:ext cx="2648738" cy="474489"/>
+          <a:off x="4476750" y="4962525"/>
+          <a:ext cx="3210815" cy="474489"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1400,7 +1424,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>captcha</a:t>
+            <a:t>captchaException</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0">
@@ -1490,8 +1514,8 @@
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>676275</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
@@ -1509,7 +1533,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2600325" y="6981825"/>
-          <a:ext cx="6991350" cy="2847975"/>
+          <a:ext cx="7696200" cy="2847975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2112,8 +2136,8 @@
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>361949</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
@@ -2131,7 +2155,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4448174" y="8820150"/>
-          <a:ext cx="4829175" cy="485775"/>
+          <a:ext cx="5505451" cy="485775"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2265,6 +2289,42 @@
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>_SESSION_KEY</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>[kaptcha</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="zh-CN" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>常量值</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>]</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="zh-CN" altLang="en-US" sz="1100">
@@ -2608,8 +2668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="S25" sqref="S25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2640,8 +2700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DFD123D-FDAB-4F21-8BCA-EE3627A19351}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>